<commit_message>
first commit on wed
</commit_message>
<xml_diff>
--- a/testData/TestCaseInputData.xlsx
+++ b/testData/TestCaseInputData.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\demoblaze_1\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB855BD-AD08-47A1-901E-317234A1E5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5083BEA-93F8-43FF-ACA5-AF53002F21CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001_DemoBlaze" sheetId="18" r:id="rId1"/>
     <sheet name="TC_002_DemoBlaze" sheetId="19" r:id="rId2"/>
     <sheet name="TC_003_DemoBlaze" sheetId="20" r:id="rId3"/>
+    <sheet name="TC_004_DemoBlaze" sheetId="21" r:id="rId4"/>
+    <sheet name="TC_005_AddToCart" sheetId="22" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>UserName</t>
   </si>
@@ -59,13 +61,63 @@
   </si>
   <si>
     <t>hjr@rj.com</t>
+  </si>
+  <si>
+    <t>ContactEmail</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>hari</t>
+  </si>
+  <si>
+    <t>msgText</t>
+  </si>
+  <si>
+    <t>message from customer naresh</t>
+  </si>
+  <si>
+    <t>message from customer -  send refund</t>
+  </si>
+  <si>
+    <t>naresh</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A3E3E"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>expName</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> expPrice</t>
+  </si>
+  <si>
+    <t>expMsg</t>
+  </si>
+  <si>
+    <t>ASUS Full HD</t>
+  </si>
+  <si>
+    <t>Product added.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$230 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +139,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A3E3E"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF292B2C"/>
+      <name val="LatoWeb"/>
     </font>
   </fonts>
   <fills count="3">
@@ -131,13 +207,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -425,13 +513,13 @@
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -447,7 +535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -470,17 +558,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -503,7 +591,7 @@
         <v>Welcome kk@mpk.com</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -528,25 +616,124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D425A79-4C4A-49CE-9EDB-8524DA6A1CBE}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="4" t="s">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA743025-8D5D-4275-B0C9-0B3425943600}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D764A4E7-B40D-403A-8776-2E48AD7ED035}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{C966664B-0DEC-4A0F-99D3-BB75EEEBCD4B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4CD88F-2056-4FF1-B87C-DC53E782EDDD}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after change in chrome version
</commit_message>
<xml_diff>
--- a/testData/TestCaseInputData.xlsx
+++ b/testData/TestCaseInputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\demoblaze_1\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA89095-21DD-4985-A9F7-E0B639874017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E2188E-EF2A-4F62-9BEE-6E1FEFC06891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="21624" windowHeight="11304" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001_DemoBlaze" sheetId="18" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="TC_003_DemoBlaze" sheetId="20" r:id="rId3"/>
     <sheet name="TC_004_DemoBlaze" sheetId="21" r:id="rId4"/>
     <sheet name="TC_005_AddToCart" sheetId="22" r:id="rId5"/>
+    <sheet name="TC_006_CartAndPurchase" sheetId="23" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>UserName</t>
   </si>
@@ -112,12 +113,69 @@
   <si>
     <t>$230 *includes tax</t>
   </si>
+  <si>
+    <t>expName</t>
+  </si>
+  <si>
+    <t>expPrice</t>
+  </si>
+  <si>
+    <t>expProductTitle</t>
+  </si>
+  <si>
+    <t>expCartFormHeaderTxt</t>
+  </si>
+  <si>
+    <t>cusName</t>
+  </si>
+  <si>
+    <t>countryName</t>
+  </si>
+  <si>
+    <t>cityName</t>
+  </si>
+  <si>
+    <t>cardNum</t>
+  </si>
+  <si>
+    <t>cardMonth</t>
+  </si>
+  <si>
+    <t>cardYear</t>
+  </si>
+  <si>
+    <t>expThankMsg</t>
+  </si>
+  <si>
+    <t>Place order</t>
+  </si>
+  <si>
+    <t>Naresh Gupta</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>234567890</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>Thank you for your purchase!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +222,17 @@
       <color rgb="FF292B2C"/>
       <name val="LatoWeb"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF292B2C"/>
+      <name val="LatoWeb"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -207,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -226,6 +295,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -510,13 +583,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -561,11 +634,11 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -620,7 +693,7 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -650,11 +723,11 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -703,15 +776,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4CD88F-2056-4FF1-B87C-DC53E782EDDD}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -739,4 +812,98 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA867F7B-C4BC-4493-8101-255E37C4433E}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L1" sqref="A1:L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="13" width="30.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>